<commit_message>
U (local): update testcases_table.xlsx
</commit_message>
<xml_diff>
--- a/Week8/Homework/testcases_table.xlsx
+++ b/Week8/Homework/testcases_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RYZEN30xx\Documents\Code\Object Oriented Programming (Python)\OOP\Week8\Homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E265A0BA-E646-403D-8ED8-F23D38B039B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC936B1-42E0-4B08-8D26-7E001E761B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{558664FD-2EC7-4EB4-B20B-2C0A812C82DA}"/>
   </bookViews>
@@ -180,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -241,16 +241,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -261,9 +281,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -280,14 +297,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -626,7 +646,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,248 +660,248 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="1:5" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="1:5" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
   </sheetData>

</xml_diff>